<commit_message>
Aggiornato excel con la statistica
</commit_message>
<xml_diff>
--- a/statistica.xlsx
+++ b/statistica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\tesi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DCF33CB-6E13-4203-87F9-A2DC20C57B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787116D9-6E27-4574-AAED-025360442A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="345" windowWidth="21600" windowHeight="11385" xr2:uid="{A81D7A3E-37BC-4C41-89C9-AF39A67B5C9E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A81D7A3E-37BC-4C41-89C9-AF39A67B5C9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -206,9 +206,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +218,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -240,15 +247,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -563,7 +573,7 @@
   <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,8 +586,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <f>22/25</f>
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="H1" t="s">
         <v>56</v>
@@ -591,8 +600,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <f>18/25</f>
-        <v>0.72</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -600,8 +608,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <f>(0+5/6)/2</f>
-        <v>0.41666666666666669</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -618,8 +625,8 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <f>23/25</f>
-        <v>0.92</v>
+        <f>24/25</f>
+        <v>0.96</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -627,15 +634,14 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <f>23/25</f>
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <f>AVERAGE(B1:B10)</f>
-        <v>0.86133333333333328</v>
+        <v>0.98000000000000009</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -643,8 +649,8 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7:B8" si="0">23/25</f>
-        <v>0.92</v>
+        <f>21/25</f>
+        <v>0.84</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -652,8 +658,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -661,8 +666,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <f>(1+5/6)/2</f>
-        <v>0.91666666666666674</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -679,8 +683,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <f>10/25</f>
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -726,9 +729,9 @@
       <c r="D17" t="s">
         <v>10</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <f>AVERAGE(B12:B47)</f>
-        <v>8.1111111111111106E-2</v>
+        <v>9.555555555555556E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -744,7 +747,8 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <f>7/25</f>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -761,8 +765,8 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <f>4/25</f>
-        <v>0.16</v>
+        <f>6/25</f>
+        <v>0.24</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -827,8 +831,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <f>9/25</f>
-        <v>0.36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -877,7 +880,8 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <f>5/25</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -885,8 +889,8 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <f>7/25</f>
-        <v>0.28000000000000003</v>
+        <f>13/25</f>
+        <v>0.52</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -894,8 +898,8 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <f>23/25</f>
-        <v>0.92</v>
+        <f>24/25</f>
+        <v>0.96</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -919,7 +923,8 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <f>11/25</f>
+        <v>0.44</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>